<commit_message>
some changes regarding to container-master-upload
</commit_message>
<xml_diff>
--- a/src/assets/Download/AddressMasterTemplate.xlsx
+++ b/src/assets/Download/AddressMasterTemplate.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7650"/>
+    <workbookView windowWidth="19635" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -19,7 +32,7 @@
     <t>manualCode</t>
   </si>
   <si>
-    <t>addressCode</t>
+    <t>address</t>
   </si>
   <si>
     <t>pincode</t>
@@ -49,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -1232,7 +1245,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>

</xml_diff>